<commit_message>
Groundwork for wrong rooms laid. You can now WAIT - how exciting!
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\SyntraZork-FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDF412-4261-49D0-90EC-C6AB4F1A3EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB88A57-DA32-4E35-935B-76E41ADF7633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{65BEF73C-3C8F-4081-879E-D0080F91A43C}"/>
+    <workbookView xWindow="28680" yWindow="3585" windowWidth="29040" windowHeight="15840" xr2:uid="{65BEF73C-3C8F-4081-879E-D0080F91A43C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
   <si>
     <t>Lobby
 0,0,0</t>
@@ -191,6 +191,60 @@
   </si>
   <si>
     <t>"~~Dog Massage for Beginners: Room 305~~\n"</t>
+  </si>
+  <si>
+    <t>-3,2,1</t>
+  </si>
+  <si>
+    <t>-2,2,1</t>
+  </si>
+  <si>
+    <t>-1,2,1</t>
+  </si>
+  <si>
+    <t>-3,2,2</t>
+  </si>
+  <si>
+    <t>-2,2,2</t>
+  </si>
+  <si>
+    <t>-1,2,2</t>
+  </si>
+  <si>
+    <t>-3,2,3</t>
+  </si>
+  <si>
+    <t>-2,2,3</t>
+  </si>
+  <si>
+    <t>-1,2,3</t>
+  </si>
+  <si>
+    <t>1,0,1</t>
+  </si>
+  <si>
+    <t>1,-1,1</t>
+  </si>
+  <si>
+    <t>1,-2,1</t>
+  </si>
+  <si>
+    <t>1,0,2</t>
+  </si>
+  <si>
+    <t>1,-1,2</t>
+  </si>
+  <si>
+    <t>1,-2,2</t>
+  </si>
+  <si>
+    <t>1,0,3</t>
+  </si>
+  <si>
+    <t>1,-1,3</t>
+  </si>
+  <si>
+    <t>1,-2,3</t>
   </si>
 </sst>
 </file>
@@ -299,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -324,6 +378,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -641,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0E6D07-4AB3-400F-AAC7-47DD26B781F1}">
   <dimension ref="B2:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -677,12 +737,21 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="30.75" customHeight="1">
+      <c r="B5" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="J5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -719,8 +788,11 @@
       <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>40</v>
@@ -731,23 +803,40 @@
       <c r="E9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="10" t="s">
         <v>35</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="30.75" customHeight="1">
       <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="30.75" customHeight="1">
+      <c r="B11" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="30.75" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -772,38 +861,58 @@
       <c r="E14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="30.75" customHeight="1">
       <c r="E15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="30.75" customHeight="1">
       <c r="E16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" ht="30.75" customHeight="1">
+      <c r="G16" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30.75" customHeight="1">
+      <c r="B17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30.75" customHeight="1">
       <c r="B18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="30.75" customHeight="1">
+    <row r="19" spans="2:7" ht="30.75" customHeight="1">
       <c r="B19" s="4" t="s">
         <v>20</v>
       </c>
@@ -817,28 +926,37 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="30.75" customHeight="1">
+    <row r="20" spans="2:7" ht="30.75" customHeight="1">
       <c r="E20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" ht="30.75" customHeight="1">
+      <c r="G20" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30.75" customHeight="1">
       <c r="E21" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" ht="30.75" customHeight="1">
+      <c r="G21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30.75" customHeight="1">
       <c r="E22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="4" t="s">
         <v>34</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some bugs fixed. Some bugs created (probably).
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\PycharmProjects\SyntraZork-FinalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB88A57-DA32-4E35-935B-76E41ADF7633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC1928B-28A6-4E4C-ADA5-5F7E907DCC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="3585" windowWidth="29040" windowHeight="15840" xr2:uid="{65BEF73C-3C8F-4081-879E-D0080F91A43C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="78">
   <si>
     <t>Lobby
 0,0,0</t>
@@ -245,6 +247,63 @@
   </si>
   <si>
     <t>1,-2,3</t>
+  </si>
+  <si>
+    <t>To implement</t>
+  </si>
+  <si>
+    <t>finish your homework</t>
+  </si>
+  <si>
+    <t>first lesson: variables (blocks of text - press enter to continue)</t>
+  </si>
+  <si>
+    <t>second lesson: functions (blocks of txt again)</t>
+  </si>
+  <si>
+    <t>break starts: go to breakroom, be back in class on time</t>
+  </si>
+  <si>
+    <t>Teachers asks a question, you should answer for POINTS</t>
+  </si>
+  <si>
+    <t>Teacher asks a question, you should answer for POINTS</t>
+  </si>
+  <si>
+    <t>wrong class</t>
+  </si>
+  <si>
+    <t>&gt; too late in class</t>
+  </si>
+  <si>
+    <t>teacher starts to explain, after 10 minutes you realise you are in the wrong class</t>
+  </si>
+  <si>
+    <t>player.thingslearned</t>
+  </si>
+  <si>
+    <t>nice-to-haves</t>
+  </si>
+  <si>
+    <t>bladder fills up 30 minutes after drink</t>
+  </si>
+  <si>
+    <t>make the wrongrooms more different</t>
+  </si>
+  <si>
+    <t>teacher will say: "make sure to return the key"</t>
+  </si>
+  <si>
+    <t>ask teacher</t>
+  </si>
+  <si>
+    <t>Breaktime</t>
+  </si>
+  <si>
+    <t>part1</t>
+  </si>
+  <si>
+    <t>part2</t>
   </si>
 </sst>
 </file>
@@ -273,7 +332,7 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,6 +342,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,12 +418,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -385,6 +447,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,7 +769,7 @@
   <dimension ref="B2:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="30.75" customHeight="1"/>
@@ -713,15 +780,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="30.75" customHeight="1">
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="30.75" customHeight="1">
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -729,7 +796,7 @@
       </c>
     </row>
     <row r="4" spans="2:10" ht="30.75" customHeight="1">
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -737,13 +804,13 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>43</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -751,13 +818,13 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="10" t="s">
         <v>31</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -765,19 +832,19 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -785,10 +852,10 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="30.75" customHeight="1">
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -799,11 +866,11 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="30.75" customHeight="1">
-      <c r="C9" s="8"/>
-      <c r="E9" s="5" t="s">
+      <c r="C9" s="7"/>
+      <c r="E9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>35</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -811,10 +878,10 @@
       </c>
     </row>
     <row r="10" spans="2:10" ht="30.75" customHeight="1">
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -822,46 +889,46 @@
       </c>
     </row>
     <row r="11" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="10" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="30.75" customHeight="1">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="30.75" customHeight="1">
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -869,10 +936,10 @@
       </c>
     </row>
     <row r="15" spans="2:10" ht="30.75" customHeight="1">
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -880,10 +947,10 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="30.75" customHeight="1">
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -891,46 +958,46 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30.75" customHeight="1">
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30.75" customHeight="1">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30.75" customHeight="1">
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30.75" customHeight="1">
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -938,10 +1005,10 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="30.75" customHeight="1">
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="10" t="s">
         <v>39</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -949,10 +1016,10 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="30.75" customHeight="1">
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>34</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -963,4 +1030,213 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA29460-F13D-4AD2-9957-D327A7B20E93}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="B1" s="11">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="C1">
+        <f>A1/B1</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" s="11">
+        <f>A1-B1</f>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4">
+        <f>B3/B1/2</f>
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="E5" s="12">
+        <v>0.82638888888888884</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="E6" s="12">
+        <v>0.84027777777777779</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" s="11">
+        <f>B8-$B$1*2</f>
+        <v>9.7222222222222224E-2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="B10" s="11">
+        <f t="shared" ref="B10:B17" si="0">B9-$B$1*2</f>
+        <v>6.9444444444444448E-2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" s="11">
+        <f>B10-B1</f>
+        <v>5.5555555555555559E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="B12" s="11">
+        <f>B11-$B$1*2</f>
+        <v>2.7777777777777783E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="B13" s="11">
+        <f>B12-$B$1*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="B14" s="11"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="B15" s="11"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BF746AC-F7D1-402F-8E16-7F34DD1B1CB3}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="F3:G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="E5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="C10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="C14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5">
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5">
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5">
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5">
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5">
+      <c r="C27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>